<commit_message>
Update R scripts and figures based on revisions
</commit_message>
<xml_diff>
--- a/graphs/S1_TableS1.xlsx
+++ b/graphs/S1_TableS1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/peter_regier_pnnl_gov/Documents/Documents/GitHub/peterregier/opti_o2/graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{278F8CA8-79BB-6A47-AFDF-40C0E729A9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:40009_{278F8CA8-79BB-6A47-AFDF-40C0E729A9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBA2A94D-5194-7A41-B92B-A2C2978E6B4A}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="230418_windowed_means" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20">
     <font>
       <sz val="12"/>
@@ -611,10 +611,10 @@
     <xf numFmtId="2" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -623,7 +623,7 @@
     <xf numFmtId="2" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -980,7 +980,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
@@ -996,10 +996,15 @@
     <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1">
+    <row r="1" spans="1:6" ht="22" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="17" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -1222,6 +1227,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>